<commit_message>
download a report via a pdf file
</commit_message>
<xml_diff>
--- a/src/assets/data/reservation00001.xlsx
+++ b/src/assets/data/reservation00001.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\education\web_2023\hotel-reservation\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCC51FD-3AD0-444A-B83B-6337E59BDF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC14EAB9-4CFD-45CD-875B-F01FCCAC695F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>max@test.ca</t>
+  </si>
+  <si>
+    <t>24/12/2023</t>
+  </si>
+  <si>
+    <t>30/12/2023</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +588,7 @@
         <v>13</v>
       </c>
       <c r="K3">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="L3" t="s">
         <v>14</v>
@@ -620,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="K4">
-        <v>234</v>
+        <v>100</v>
       </c>
       <c r="L4" t="s">
         <v>10</v>
@@ -658,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="K5">
-        <v>234</v>
+        <v>135</v>
       </c>
       <c r="L5" t="s">
         <v>10</v>
@@ -696,9 +702,47 @@
         <v>13</v>
       </c>
       <c r="K6">
-        <v>234</v>
+        <v>306</v>
       </c>
       <c r="L6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>203</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45211</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7">
+        <v>250</v>
+      </c>
+      <c r="L7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -714,6 +758,8 @@
     <hyperlink ref="G4" r:id="rId8" xr:uid="{4278EF47-60D0-45D3-B82E-2189CEB68134}"/>
     <hyperlink ref="G5" r:id="rId9" xr:uid="{75123E23-D0C3-49DD-AF4D-2C40FFBD6582}"/>
     <hyperlink ref="G6" r:id="rId10" xr:uid="{9C4BE6C2-9882-4057-859A-C013D6BBB6C6}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{36B415B6-EBFF-455F-A737-DE1D073C4EAD}"/>
+    <hyperlink ref="G7" r:id="rId12" xr:uid="{7DB19603-0DFA-408B-88A5-9DD54FF1358E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>